<commit_message>
Arreglo de errores en mensajes mas implementacion de mas validaciones y mejora en unas interfaces
</commit_message>
<xml_diff>
--- a/Main/Archivos/Archivos_Stock/reporte_stock.xlsx
+++ b/Main/Archivos/Archivos_Stock/reporte_stock.xlsx
@@ -525,7 +525,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>36</t>
         </is>
       </c>
     </row>
@@ -552,7 +552,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>18</t>
         </is>
       </c>
     </row>

</xml_diff>